<commit_message>
combine routing and scheduling
</commit_message>
<xml_diff>
--- a/Input data/Task_list_Test.xlsx
+++ b/Input data/Task_list_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lichen/PycharmProjects/ACO_Example/Input data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33847A13-B699-8944-A1D7-E84A0FE49D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BC8334-0A10-1041-8EB8-B15C32385BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="6520" windowWidth="27440" windowHeight="16940" xr2:uid="{A42DF498-1344-D146-AA3B-A40409BEB30C}"/>
+    <workbookView xWindow="1360" yWindow="1060" windowWidth="27440" windowHeight="16940" xr2:uid="{A42DF498-1344-D146-AA3B-A40409BEB30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasklist" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Task type</t>
   </si>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD6D0D4-69AF-C543-B15F-FC934284425F}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -790,6 +790,296 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>225</v>
+      </c>
+      <c r="D12" s="1">
+        <v>57</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>285</v>
+      </c>
+      <c r="G12" s="1">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>225</v>
+      </c>
+      <c r="D13" s="1">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>100</v>
+      </c>
+      <c r="G13" s="1">
+        <v>141</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>370</v>
+      </c>
+      <c r="G14" s="1">
+        <v>93</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>400</v>
+      </c>
+      <c r="G15" s="1">
+        <v>100</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>225</v>
+      </c>
+      <c r="D16" s="1">
+        <v>57</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>200</v>
+      </c>
+      <c r="G16" s="1">
+        <v>146</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>225</v>
+      </c>
+      <c r="D17" s="1">
+        <v>57</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>285</v>
+      </c>
+      <c r="G17" s="1">
+        <v>72</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>225</v>
+      </c>
+      <c r="D18" s="1">
+        <v>57</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>100</v>
+      </c>
+      <c r="G18" s="1">
+        <v>141</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>370</v>
+      </c>
+      <c r="G19" s="1">
+        <v>93</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>400</v>
+      </c>
+      <c r="G20" s="1">
+        <v>100</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>225</v>
+      </c>
+      <c r="D21" s="1">
+        <v>57</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>200</v>
+      </c>
+      <c r="G21" s="1">
+        <v>146</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>